<commit_message>
DDL Scripts for Staging tables
Bringing up the tables for staging the merged data for two months
</commit_message>
<xml_diff>
--- a/Changelog.xlsx
+++ b/Changelog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace\Personal Projects\Bellabeats Fitness Tracker Analytics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace\Personal Projects\Bellabeat Fitness Tracker Analytics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA14AE95-DEB1-49A2-8C3F-1DFFC626847C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E656FF76-CC5A-4E1E-8454-8BC411D4F5F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14169" xr2:uid="{BCB204A5-C604-4E75-A162-3AA5892C8ABF}"/>
   </bookViews>
@@ -545,10 +545,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
Analyze and Visualize using Tableau
Worksheets, Dashboards and Storyboards updated.
Story title font: Lucida Calligraphy. RGB (73,152,148)
Story navigator font: Leelawadee UI. RGB (51,51,51)
</commit_message>
<xml_diff>
--- a/Changelog.xlsx
+++ b/Changelog.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace\Personal Projects\Bellabeat Fitness Tracker Analytics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E656FF76-CC5A-4E1E-8454-8BC411D4F5F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1F8FE80-A88C-45A1-8A6E-7CC1BC0548A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14169" xr2:uid="{BCB204A5-C604-4E75-A162-3AA5892C8ABF}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14169" activeTab="2" xr2:uid="{BCB204A5-C604-4E75-A162-3AA5892C8ABF}"/>
   </bookViews>
   <sheets>
     <sheet name="Changelog" sheetId="3" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="59">
   <si>
     <t>Date</t>
   </si>
@@ -407,6 +408,42 @@
 Value indicating the sleep state. 
 1 = asleep, 2 = restless, 3 = awake </t>
     </r>
+  </si>
+  <si>
+    <t>Most Active Days</t>
+  </si>
+  <si>
+    <t>Most Inactive days</t>
+  </si>
+  <si>
+    <t>Average Calories burned per day</t>
+  </si>
+  <si>
+    <t>Caloeries outliers analysis</t>
+  </si>
+  <si>
+    <t>Healthy sleep days</t>
+  </si>
+  <si>
+    <t>Unhealthy sleep days</t>
+  </si>
+  <si>
+    <t>People who sleep more than once a day</t>
+  </si>
+  <si>
+    <t>Sleeping pattern of those people and split of sleep each time</t>
+  </si>
+  <si>
+    <t>Calories burned to weight lost analysis</t>
+  </si>
+  <si>
+    <t>Activity split per day</t>
+  </si>
+  <si>
+    <t>Most Active time of day</t>
+  </si>
+  <si>
+    <t>Most Sedentary time of</t>
   </si>
 </sst>
 </file>
@@ -866,9 +903,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7CEFA53-FC8F-422B-9520-A6B40A488A62}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1422,4 +1459,83 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18C4FAFC-02EB-42F1-B39B-373D89F665E3}">
+  <dimension ref="A2:B14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="53.875" customWidth="1"/>
+    <col min="2" max="2" width="81.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>